<commit_message>
finaly add shift algorythm
</commit_message>
<xml_diff>
--- a/doc/math.xlsx
+++ b/doc/math.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\workspace\MAGmapper\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC29E96-4523-46B7-8BF5-E18AC1BD7F99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF353B-0D39-4E8B-B9C4-15BB204C83CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="4800" xr2:uid="{0D4A8800-F206-4052-A30E-9BA1ECB82C42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stable" sheetId="1" r:id="rId1"/>
+    <sheet name="hypothetic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -59,6 +60,30 @@
   <si>
     <t>add</t>
   </si>
+  <si>
+    <t>item-length</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>preset</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Length-float</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>right+D16C18:E18:G19</t>
+  </si>
 </sst>
 </file>
 
@@ -81,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +131,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -119,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -128,6 +159,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -209,7 +242,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$K$22:$K$37</c:f>
+              <c:f>Stable!$K$22:$K$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -266,7 +299,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$22:$L$37</c:f>
+              <c:f>Stable!$L$22:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -286,37 +319,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>1.1111111111111112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>1.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>2.4444444444444446</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>3.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>2.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,7 +388,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$22:$B$37</c:f>
+              <c:f>Stable!$B$22:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -412,7 +445,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$22:$C$37</c:f>
+              <c:f>Stable!$C$22:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -471,6 +504,540 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-D23D-4D99-857C-C58F9257A54B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="585144752"/>
+        <c:axId val="585145080"/>
+        <c:extLst/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="585144752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585145080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="585145080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="585144752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="5000"/>
+              <a:lumOff val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="74000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="45000"/>
+              <a:lumOff val="55000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="83000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="45000"/>
+              <a:lumOff val="55000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="30000"/>
+              <a:lumOff val="70000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.4138905713708862E-2"/>
+          <c:y val="6.1213778810634237E-2"/>
+          <c:w val="0.91845376165586134"/>
+          <c:h val="0.85291061439313265"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:schemeClr val="bg1"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Stable!$K$22:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Stable!$L$22:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.4444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C7B-498C-A26D-8FD3FAC959C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Stable!$B$22:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Stable!$C$22:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C7B-498C-A26D-8FD3FAC959C3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -716,7 +1283,560 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1257,6 +2377,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{548331D1-58CE-476B-B164-5F604E42A8F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1570,10 +2733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D6DDA9-03B4-40EF-99B7-0A7449601F04}">
-  <dimension ref="A3:L37"/>
+  <dimension ref="A3:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,126 +2751,153 @@
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <f>B5/B4</f>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+      <c r="L9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="L10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="L12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="M12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7">
+        <f>C25-C22</f>
+        <v>3</v>
+      </c>
+      <c r="L14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <f>C37-C22</f>
+        <v>3</v>
+      </c>
+      <c r="L15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="1"/>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1715,12 +2905,6 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
         <v>1</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -1738,18 +2922,18 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>D22+$C$11</f>
+        <f>D22+$B$11</f>
         <v>0</v>
       </c>
       <c r="D22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <f>B22*$C$8+$C$10</f>
+        <f>B22*$B$7/$B$12+$B$10</f>
         <v>1</v>
       </c>
       <c r="G22" s="4">
-        <f>C22*$F$8+$F$10</f>
+        <f>C22*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K22" s="2">
@@ -1766,18 +2950,18 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>D23+$C$11</f>
+        <f>D23+$B$11</f>
         <v>1</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="F23" s="4">
-        <f>B23*$C$8+$C$10</f>
+        <f t="shared" ref="F23:F37" si="0">B23*$B$7/$B$12+$B$10</f>
         <v>1</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" ref="G23:G37" si="0">C23*$F$8+$F$10</f>
+        <f>C23*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K23" s="2">
@@ -1785,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L22:L37" si="2">C23*F23</f>
+        <f t="shared" ref="L23:L37" si="2">C23*F23</f>
         <v>1</v>
       </c>
     </row>
@@ -1797,18 +2981,18 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>D24+$C$11</f>
+        <f>D24+$B$11</f>
         <v>2</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" ref="F22:F37" si="3">B24*$C$8+$C$10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="0"/>
+        <f>C24*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K24" s="2">
@@ -1825,18 +3009,18 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>D25+$C$11</f>
+        <f>D25+$B$11</f>
         <v>3</v>
       </c>
       <c r="D25" s="3">
         <v>3</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
+        <f>C25*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K25" s="2">
@@ -1853,18 +3037,18 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>D26+$C$11</f>
+        <f>D26+$B$11</f>
         <v>0</v>
       </c>
       <c r="D26" s="3">
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="0"/>
+        <f>C26*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K26" s="2">
@@ -1881,18 +3065,18 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <f>D27+$C$11</f>
+        <f>D27+$B$11</f>
         <v>1</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="0"/>
+        <f>C27*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K27" s="2">
@@ -1901,7 +3085,7 @@
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1909,18 +3093,18 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <f>D28+$C$11</f>
+        <f>D28+$B$11</f>
         <v>2</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="0"/>
+        <f>C28*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K28" s="2">
@@ -1929,7 +3113,7 @@
       </c>
       <c r="L28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2.2222222222222223</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1937,18 +3121,18 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <f>D29+$C$11</f>
+        <f>D29+$B$11</f>
         <v>3</v>
       </c>
       <c r="D29" s="3">
         <v>3</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="3"/>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.1111111111111112</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="0"/>
+        <f>C29*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K29" s="2">
@@ -1957,7 +3141,7 @@
       </c>
       <c r="L29">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1968,18 +3152,18 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <f>D30+$C$11</f>
+        <f>D30+$B$11</f>
         <v>0</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.2222222222222223</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="0"/>
+        <f>C30*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K30" s="2">
@@ -1996,18 +3180,18 @@
         <v>2</v>
       </c>
       <c r="C31">
-        <f>D31+$C$11</f>
+        <f>D31+$B$11</f>
         <v>1</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.2222222222222223</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="0"/>
+        <f>C31*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K31" s="2">
@@ -2016,7 +3200,7 @@
       </c>
       <c r="L31">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.2222222222222223</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2027,18 +3211,18 @@
         <v>2</v>
       </c>
       <c r="C32">
-        <f>D32+$C$11</f>
+        <f>D32+$B$11</f>
         <v>2</v>
       </c>
       <c r="D32" s="3">
         <v>2</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.2222222222222223</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="0"/>
+        <f>C32*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K32" s="2">
@@ -2047,7 +3231,7 @@
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2.4444444444444446</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2055,18 +3239,18 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <f>D33+$C$11</f>
+        <f>D33+$B$11</f>
         <v>3</v>
       </c>
       <c r="D33" s="3">
         <v>3</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.2222222222222223</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="0"/>
+        <f>C33*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K33" s="2">
@@ -2075,7 +3259,7 @@
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
@@ -2083,18 +3267,18 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <f>D34+$C$11</f>
+        <f>D34+$B$11</f>
         <v>0</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="3"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="G34" s="4">
-        <f t="shared" si="0"/>
+        <f>C34*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K34" s="2">
@@ -2111,18 +3295,18 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <f>D35+$C$11</f>
+        <f>D35+$B$11</f>
         <v>1</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" si="3"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="G35" s="4">
-        <f t="shared" si="0"/>
+        <f>C35*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K35" s="2">
@@ -2131,7 +3315,7 @@
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
@@ -2139,18 +3323,18 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <f>D36+$C$11</f>
+        <f>D36+$B$11</f>
         <v>2</v>
       </c>
       <c r="D36" s="3">
         <v>2</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" si="3"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="G36" s="4">
-        <f t="shared" si="0"/>
+        <f>C36*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K36" s="2">
@@ -2159,7 +3343,7 @@
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -2167,18 +3351,18 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <f>D37+$C$11</f>
+        <f>D37+$B$11</f>
         <v>3</v>
       </c>
       <c r="D37" s="3">
         <v>3</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" si="3"/>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" si="0"/>
+        <f>C37*$M$12+$M$14</f>
         <v>1</v>
       </c>
       <c r="K37" s="2">
@@ -2187,7 +3371,773 @@
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1CA48D-EA0D-447F-9F95-5F0F61EB112D}">
+  <dimension ref="A3:O57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <f>B5/B4</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="N9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+      <c r="N10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <f>C25-C22</f>
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="N12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <f>C37-C22</f>
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>B7*B13</f>
+        <v>6</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H19" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>C42+$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>$B$15+B22</f>
+        <v>6</v>
+      </c>
+      <c r="H22" s="9">
+        <f>B22*$B$7+$B$8</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <f>C22*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <f>B22*I22</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>C22*H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>C43+$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E37" si="0">$B$15+B23</f>
+        <v>6</v>
+      </c>
+      <c r="H23" s="9">
+        <f>B23*$B$7+$B$8</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <f>C23*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" ref="M23:M37" si="1">B23*I23</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>C23*H23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>C44+$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H24" s="9">
+        <f>B24*$B$7+$B$8</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <f>C24*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>C24*H24</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>C45+$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H25" s="9">
+        <f>B25*$B$7+$B$8</f>
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <f>C25*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>C25*H25</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f>C46+$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H26" s="9">
+        <f>B26*$B$7+$B$8</f>
+        <v>3</v>
+      </c>
+      <c r="I26" s="9">
+        <f>C26*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <f>C26*H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f>C47+$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H27" s="9">
+        <f>B27*$B$7+$B$8</f>
+        <v>3</v>
+      </c>
+      <c r="I27" s="9">
+        <f>C27*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <f>C27*H27</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>C48+$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H28" s="9">
+        <f>B28*$B$7+$B$8</f>
+        <v>3</v>
+      </c>
+      <c r="I28" s="9">
+        <f>C28*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f>C28*H28</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f>C49+$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H29" s="9">
+        <f>B29*$B$7+$B$8</f>
+        <v>3</v>
+      </c>
+      <c r="I29" s="9">
+        <f>C29*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f>C29*H29</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <f>C50+$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H30" s="9">
+        <f>B30*$B$7+$B$8</f>
+        <v>5</v>
+      </c>
+      <c r="I30" s="9">
+        <f>C30*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <f>C30*H30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <f>C51+$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H31" s="9">
+        <f>B31*$B$7+$B$8</f>
+        <v>5</v>
+      </c>
+      <c r="I31" s="9">
+        <f>C31*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <f>C31*H31</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f>C52+$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H32" s="9">
+        <f>B32*$B$7+$B$8</f>
+        <v>5</v>
+      </c>
+      <c r="I32" s="9">
+        <f>C32*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <f>C32*H32</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f>C53+$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H33" s="9">
+        <f>B33*$B$7+$B$8</f>
+        <v>5</v>
+      </c>
+      <c r="I33" s="9">
+        <f>C33*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <f>C33*H33</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <f>C54+$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H34" s="9">
+        <f>B34*$B$7+$B$8</f>
+        <v>7</v>
+      </c>
+      <c r="I34" s="9">
+        <f>C34*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <f>C34*H34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <f>C55+$B$9</f>
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H35" s="9">
+        <f>B35*$B$7+$B$8</f>
+        <v>7</v>
+      </c>
+      <c r="I35" s="9">
+        <f>C35*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N35">
+        <f>C35*H35</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f>C56+$B$9</f>
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H36" s="9">
+        <f>B36*$B$7+$B$8</f>
+        <v>7</v>
+      </c>
+      <c r="I36" s="9">
+        <f>C36*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N36">
+        <f>C36*H36</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f>C57+$B$9</f>
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H37" s="9">
+        <f>B37*$B$7+$B$8</f>
+        <v>7</v>
+      </c>
+      <c r="I37" s="9">
+        <f>C37*$O$12+$O$14</f>
+        <v>1</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N37">
+        <f>C37*H37</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C48" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed code & tests for uv mapping
</commit_message>
<xml_diff>
--- a/doc/math.xlsx
+++ b/doc/math.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\workspace\MAGmapper\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF353B-0D39-4E8B-B9C4-15BB204C83CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2193E5DB-FDA0-44E5-A2C7-AAF9AAE811DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="4800" xr2:uid="{0D4A8800-F206-4052-A30E-9BA1ECB82C42}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="4800" activeTab="1" xr2:uid="{0D4A8800-F206-4052-A30E-9BA1ECB82C42}"/>
   </bookViews>
   <sheets>
     <sheet name="Stable" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>x</t>
   </si>
@@ -70,26 +70,53 @@
     <t>height</t>
   </si>
   <si>
-    <t>preset</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>Length-float</t>
-  </si>
-  <si>
     <t>length</t>
   </si>
   <si>
-    <t>right+D16C18:E18:G19</t>
+    <t>vertices</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>tl</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>faktor x</t>
+  </si>
+  <si>
+    <t>faktor y</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>faktor -1</t>
+  </si>
+  <si>
+    <t>delta part</t>
+  </si>
+  <si>
+    <t>faktor für y</t>
+  </si>
+  <si>
+    <t>size x</t>
+  </si>
+  <si>
+    <t>size y</t>
+  </si>
+  <si>
+    <t>faktor für x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +132,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,12 +168,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -146,11 +187,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -159,8 +215,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -262,37 +326,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -319,37 +383,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1111111111111112</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2222222222222223</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4444444444444446</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.666666666666667</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.3333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,20 +797,169 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4138905713708862E-2"/>
-          <c:y val="6.1213778810634237E-2"/>
-          <c:w val="0.91845376165586134"/>
-          <c:h val="0.85291061439313265"/>
+          <c:x val="4.0340265159162801E-2"/>
+          <c:y val="1.6242913384347642E-2"/>
+          <c:w val="0.9374471139825471"/>
+          <c:h val="0.90170597414652787"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>t3</c:v>
+            <c:v>Basic Vertices</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>hypothetic!$B$18:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>hypothetic!$C$18:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-87FB-44E1-8772-9AFA5FABEC4C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>result</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -760,161 +973,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:schemeClr val="bg1"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Stable!$K$22:$K$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Stable!$L$22:$L$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1111111111111112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2222222222222223</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3333333333333335</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2222222222222223</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.4444444444444446</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.6666666666666665</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C7B-498C-A26D-8FD3FAC959C3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -922,7 +985,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Stable!$B$22:$B$37</c:f>
+              <c:f>hypothetic!$T$18:$T$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -942,44 +1005,44 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.1111111111111112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>1.2222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>2.4444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>2.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>3.6666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Stable!$C$22:$C$37</c:f>
+              <c:f>hypothetic!$U$18:$U$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -999,37 +1062,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>1.1111111111111112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.3333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>1.2222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>2.4444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>3.6666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>2.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,7 +1100,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3C7B-498C-A26D-8FD3FAC959C3}"/>
+              <c16:uniqueId val="{00000001-87FB-44E1-8772-9AFA5FABEC4C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1284,10 +1347,10 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2397,16 +2460,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2735,8 +2798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D6DDA9-03B4-40EF-99B7-0A7449601F04}">
   <dimension ref="A3:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2791,7 +2854,7 @@
       </c>
       <c r="B7" s="7">
         <f>B5/B4</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -2823,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2839,7 +2902,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="7">
         <v>3</v>
@@ -2852,7 +2915,8 @@
         <v>8</v>
       </c>
       <c r="M12" s="7">
-        <v>0</v>
+        <f>M10/M9</f>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2896,9 +2960,6 @@
       <c r="F19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -2906,6 +2967,12 @@
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>0</v>
@@ -2922,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>D22+$B$11</f>
+        <f t="shared" ref="C22:C37" si="0">D22+$B$11</f>
         <v>0</v>
       </c>
       <c r="D22" s="3">
@@ -2950,26 +3017,26 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>D23+$B$11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" ref="F23:F37" si="0">B23*$B$7/$B$12+$B$10</f>
+        <f t="shared" ref="F23:F37" si="1">B23*$B$7/$B$12+$B$10</f>
         <v>1</v>
       </c>
       <c r="G23" s="4">
-        <f>C23*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" ref="G22:G37" si="2">C23*$M$12+$M$14</f>
+        <v>4</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" ref="K23:K37" si="1">B23*G23</f>
+        <f t="shared" ref="K23:K37" si="3">B23*G23</f>
         <v>0</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L23:L37" si="2">C23*F23</f>
+        <f t="shared" ref="L23:L37" si="4">C23*F23</f>
         <v>1</v>
       </c>
     </row>
@@ -2981,26 +3048,26 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>D24+$B$11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G24" s="4">
-        <f>C24*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -3009,26 +3076,26 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>D25+$B$11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D25" s="3">
         <v>3</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G25" s="4">
-        <f>C25*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -3037,26 +3104,26 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>D26+$B$11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D26" s="3">
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G26" s="4">
-        <f>C26*$M$12+$M$14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3065,27 +3132,27 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <f>D27+$B$11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G27" s="4">
-        <f>C27*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="L27">
-        <f t="shared" si="2"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3093,27 +3160,27 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <f>D28+$B$11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D28" s="3">
         <v>2</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G28" s="4">
-        <f>C28*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="L28">
-        <f t="shared" si="2"/>
-        <v>2.2222222222222223</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3121,27 +3188,27 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <f>D29+$B$11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D29" s="3">
         <v>3</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G29" s="4">
-        <f>C29*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="L29">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333335</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3152,26 +3219,26 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <f>D30+$B$11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G30" s="4">
-        <f>C30*$M$12+$M$14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3180,27 +3247,27 @@
         <v>2</v>
       </c>
       <c r="C31">
-        <f>D31+$B$11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G31" s="4">
-        <f>C31*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="L31">
-        <f t="shared" si="2"/>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3211,27 +3278,27 @@
         <v>2</v>
       </c>
       <c r="C32">
-        <f>D32+$B$11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D32" s="3">
         <v>2</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G32" s="4">
-        <f>C32*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="4"/>
         <v>2</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>2.4444444444444446</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -3239,27 +3306,27 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <f>D33+$B$11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D33" s="3">
         <v>3</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2222222222222223</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G33" s="4">
-        <f>C33*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>20</v>
       </c>
       <c r="L33">
-        <f t="shared" si="2"/>
-        <v>3.666666666666667</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
@@ -3267,26 +3334,26 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <f>D34+$B$11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G34" s="4">
-        <f>C34*$M$12+$M$14</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3295,27 +3362,27 @@
         <v>3</v>
       </c>
       <c r="C35">
-        <f>D35+$B$11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D35" s="3">
         <v>1</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G35" s="4">
-        <f>C35*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="L35">
-        <f t="shared" si="2"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
@@ -3323,27 +3390,27 @@
         <v>3</v>
       </c>
       <c r="C36">
-        <f>D36+$B$11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D36" s="3">
         <v>2</v>
       </c>
       <c r="F36" s="4">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G36" s="4">
-        <f>C36*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>21</v>
       </c>
       <c r="L36">
-        <f t="shared" si="2"/>
-        <v>2.6666666666666665</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -3351,27 +3418,27 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <f>D37+$B$11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D37" s="3">
         <v>3</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G37" s="4">
-        <f>C37*$M$12+$M$14</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="4"/>
         <v>3</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3383,762 +3450,1378 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1CA48D-EA0D-447F-9F95-5F0F61EB112D}">
-  <dimension ref="A3:O57"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="4.85546875" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="21" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="1"/>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>C2/C33</f>
+        <v>1.3333333333333333</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="7">
-        <f>B5/B4</f>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>C3/B33</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="F17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="T17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="F18">
+        <f>B18/($C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <f>($C$6-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H18">
+        <f>G18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>H18+1</f>
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f>C18/$C$13</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="10">
+        <f>($C$7-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N18">
+        <f>M18*L18</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>N18+1</f>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="T18" s="10">
+        <f>B18*O18</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="10">
+        <f>C18*I18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="F19">
+        <f>B19/($C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" ref="G19:G33" si="0">($C$6-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H33" si="1">G19*F19</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I33" si="2">H19+1</f>
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ref="L19:L33" si="3">C19/$C$13</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" ref="M19:M33" si="4">($C$7-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:N33" si="5">M19*L19</f>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O33" si="6">N19+1</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="T19" s="10">
+        <f t="shared" ref="T19:T33" si="7">B19*O19</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="10">
+        <f>C19*I19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10">
         <v>2</v>
       </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1"/>
-      <c r="N8" s="1" t="s">
+      <c r="D20" s="3"/>
+      <c r="F20">
+        <f t="shared" ref="F19:F33" si="8">B20/($C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <f>($C$6-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H20">
+        <f>G20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M20" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="T20" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="10">
+        <f>C20*I20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
         <v>3</v>
       </c>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="N9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J10" s="1"/>
-      <c r="N10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J11" s="1"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7">
-        <f>C25-C22</f>
+      <c r="D21" s="3"/>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q21" s="8"/>
+      <c r="T21" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="10">
+        <f>C21*I21</f>
         <v>3</v>
       </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="N12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7">
-        <f>C37-C22</f>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="F22">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q22" s="3"/>
+      <c r="T22" s="10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U22" s="10">
+        <f>C22*I22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="F23">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G23" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M23" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="Q23" s="3"/>
+      <c r="T23" s="10">
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="U23" s="10">
+        <f>C23*I23</f>
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="F24">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G24" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H24">
+        <f>G24*F24</f>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M24" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="Q24" s="3"/>
+      <c r="T24" s="10">
+        <f t="shared" si="7"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="U24" s="10">
+        <f>C24*I24</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="10">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f>B7*B13</f>
-        <v>6</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H19" s="8" t="s">
+      <c r="D25" s="3"/>
+      <c r="F25">
+        <f t="shared" si="8"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M25" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q25" s="3"/>
+      <c r="T25" s="10">
+        <f t="shared" si="7"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="U25" s="10">
+        <f>C25*I25</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="10">
         <v>2</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="F26">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G26" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" s="3"/>
+      <c r="T26" s="10">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="U26" s="10">
+        <f>C26*I26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="10">
+        <v>2</v>
+      </c>
+      <c r="C27" s="10">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="F27">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G27" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M27" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="6"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="Q27" s="3"/>
+      <c r="T27" s="10">
+        <f t="shared" si="7"/>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="U27" s="10">
+        <f>C27*I27</f>
+        <v>1.2222222222222221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="10">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="F28">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G28" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M28" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="Q28" s="3"/>
+      <c r="T28" s="10">
+        <f t="shared" si="7"/>
+        <v>2.4444444444444442</v>
+      </c>
+      <c r="U28" s="10">
+        <f>C28*I28</f>
+        <v>2.4444444444444442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f>C42+$B$9</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f>$B$15+B22</f>
-        <v>6</v>
-      </c>
-      <c r="H22" s="9">
-        <f>B22*$B$7+$B$8</f>
-        <v>1</v>
-      </c>
-      <c r="I22" s="9">
-        <f>C22*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M22" s="2">
-        <f>B22*I22</f>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f>C22*H22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f>C43+$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f t="shared" ref="E23:E37" si="0">$B$15+B23</f>
-        <v>6</v>
-      </c>
-      <c r="H23" s="9">
-        <f>B23*$B$7+$B$8</f>
-        <v>1</v>
-      </c>
-      <c r="I23" s="9">
-        <f>C23*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M23" s="2">
-        <f t="shared" ref="M23:M37" si="1">B23*I23</f>
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <f>C23*H23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <f>C44+$B$9</f>
+      <c r="D29" s="3"/>
+      <c r="F29">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G29" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M29" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q29" s="3"/>
+      <c r="T29" s="10">
+        <f t="shared" si="7"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="U29" s="10">
+        <f>C29*I29</f>
+        <v>3.6666666666666661</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
+        <v>3</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="F30">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q30" s="3"/>
+      <c r="T30" s="10">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="U30" s="10">
+        <f>C30*I30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="10">
+        <v>3</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="F31">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G31" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M31" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>0.11111111111111108</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="Q31" s="3"/>
+      <c r="T31" s="10">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="U31" s="10">
+        <f>C31*I31</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="10">
+        <v>3</v>
+      </c>
+      <c r="C32" s="10">
         <v>2</v>
       </c>
-      <c r="E24">
+      <c r="D32" s="3"/>
+      <c r="F32">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H24" s="9">
-        <f>B24*$B$7+$B$8</f>
-        <v>1</v>
-      </c>
-      <c r="I24" s="9">
-        <f>C24*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M24" s="2">
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <f>C24*H24</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f>C45+$B$9</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M32" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>0.22222222222222215</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="6"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="Q32" s="3"/>
+      <c r="T32" s="10">
+        <f t="shared" si="7"/>
+        <v>3.6666666666666661</v>
+      </c>
+      <c r="U32" s="10">
+        <f>C32*I32</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="9">
         <v>3</v>
       </c>
-      <c r="E25">
+      <c r="C33" s="9">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="F33">
+        <f>B33/($C$12)</f>
+        <v>1</v>
+      </c>
+      <c r="G33" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H25" s="9">
-        <f>B25*$B$7+$B$8</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="9">
-        <f>C25*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M25" s="2">
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <f>C25*H25</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <f>C46+$B$9</f>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H26" s="9">
-        <f>B26*$B$7+$B$8</f>
-        <v>3</v>
-      </c>
-      <c r="I26" s="9">
-        <f>C26*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M26" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <f>C26*H26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f>C47+$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H27" s="9">
-        <f>B27*$B$7+$B$8</f>
-        <v>3</v>
-      </c>
-      <c r="I27" s="9">
-        <f>C27*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M27" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <f>C27*H27</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <f>C48+$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H28" s="9">
-        <f>B28*$B$7+$B$8</f>
-        <v>3</v>
-      </c>
-      <c r="I28" s="9">
-        <f>C28*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <f>C28*H28</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f>C49+$B$9</f>
-        <v>3</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H29" s="9">
-        <f>B29*$B$7+$B$8</f>
-        <v>3</v>
-      </c>
-      <c r="I29" s="9">
-        <f>C29*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <f>C29*H29</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M33" s="10">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Q33" s="3"/>
+      <c r="T33" s="10">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="B30" s="3">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <f>C50+$B$9</f>
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H30" s="9">
-        <f>B30*$B$7+$B$8</f>
-        <v>5</v>
-      </c>
-      <c r="I30" s="9">
-        <f>C30*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N30">
-        <f>C30*H30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="3">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <f>C51+$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H31" s="9">
-        <f>B31*$B$7+$B$8</f>
-        <v>5</v>
-      </c>
-      <c r="I31" s="9">
-        <f>C31*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N31">
-        <f>C31*H31</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <f>C52+$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H32" s="9">
-        <f>B32*$B$7+$B$8</f>
-        <v>5</v>
-      </c>
-      <c r="I32" s="9">
-        <f>C32*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M32" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N32">
-        <f>C32*H32</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>2</v>
-      </c>
-      <c r="C33">
-        <f>C53+$B$9</f>
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H33" s="9">
-        <f>B33*$B$7+$B$8</f>
-        <v>5</v>
-      </c>
-      <c r="I33" s="9">
-        <f>C33*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M33" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N33">
-        <f>C33*H33</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <f>C54+$B$9</f>
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H34" s="9">
-        <f>B34*$B$7+$B$8</f>
-        <v>7</v>
-      </c>
-      <c r="I34" s="9">
-        <f>C34*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M34" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N34">
-        <f>C34*H34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <f>C55+$B$9</f>
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H35" s="9">
-        <f>B35*$B$7+$B$8</f>
-        <v>7</v>
-      </c>
-      <c r="I35" s="9">
-        <f>C35*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M35" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N35">
-        <f>C35*H35</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="3">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <f>C56+$B$9</f>
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H36" s="9">
-        <f>B36*$B$7+$B$8</f>
-        <v>7</v>
-      </c>
-      <c r="I36" s="9">
-        <f>C36*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M36" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N36">
-        <f>C36*H36</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="3">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <f>C57+$B$9</f>
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H37" s="9">
-        <f>B37*$B$7+$B$8</f>
-        <v>7</v>
-      </c>
-      <c r="I37" s="9">
-        <f>C37*$O$12+$O$14</f>
-        <v>1</v>
-      </c>
-      <c r="M37" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N37">
-        <f>C37*H37</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C42" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C43" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C44" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C45" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C46" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C47" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C48" s="3">
-        <v>2</v>
-      </c>
+      <c r="U33" s="10">
+        <f>C33*I33</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C48" s="3"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="3">
-        <v>3</v>
-      </c>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="3">
-        <v>0</v>
-      </c>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="3">
-        <v>1</v>
-      </c>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="3">
-        <v>2</v>
-      </c>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="3">
-        <v>3</v>
-      </c>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="3">
-        <v>0</v>
-      </c>
+      <c r="C54" s="3"/>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="3">
-        <v>1</v>
-      </c>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="3">
-        <v>2</v>
-      </c>
+      <c r="C56" s="3"/>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" s="3">
-        <v>3</v>
-      </c>
+      <c r="C57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>